<commit_message>
20190930 - Microspot iPhone color mapping
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -164,18 +164,12 @@
     <t>ProductFamily</t>
   </si>
   <si>
-    <t>iphone</t>
-  </si>
-  <si>
     <t>\Data\Output\PriceComparison.xlsx</t>
   </si>
   <si>
     <t>Excel file with price comparison</t>
   </si>
   <si>
-    <t>Name of the product family to compare</t>
-  </si>
-  <si>
     <t>https://www.mediamarkt.ch/fr/</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>EmailSubject</t>
   </si>
   <si>
-    <t>Price Comparison:</t>
-  </si>
-  <si>
     <t>Email subject</t>
   </si>
   <si>
@@ -224,46 +215,22 @@
     <t>EmailSender</t>
   </si>
   <si>
-    <t>SMTP_Server</t>
-  </si>
-  <si>
-    <t>SMTP_Port</t>
-  </si>
-  <si>
-    <t>smtp.gmail.com</t>
-  </si>
-  <si>
-    <t>thuannn@gmail.com</t>
-  </si>
-  <si>
-    <t>SMTP_Password</t>
-  </si>
-  <si>
-    <t>ExchangeDomain</t>
-  </si>
-  <si>
-    <t>swordgroup</t>
-  </si>
-  <si>
-    <t>ExchangePassword</t>
-  </si>
-  <si>
     <t>EmailReceiver</t>
   </si>
   <si>
-    <t>ExchangeUser</t>
-  </si>
-  <si>
-    <t>BaoTran2015$$</t>
-  </si>
-  <si>
-    <t>tnguyen</t>
-  </si>
-  <si>
-    <t>SMTP_User</t>
-  </si>
-  <si>
     <t>ProductSearchLimit</t>
+  </si>
+  <si>
+    <t>Name of the product family to compare. Use plus sign (+) to refine search results.</t>
+  </si>
+  <si>
+    <t>Number of products to compare</t>
+  </si>
+  <si>
+    <t>Price Comparison</t>
+  </si>
+  <si>
+    <t>iphone 11</t>
   </si>
 </sst>
 </file>
@@ -594,15 +561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z991"/>
+  <dimension ref="A1:Z983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.5703125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
@@ -660,153 +627,110 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1764,14 +1688,6 @@
     <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>